<commit_message>
Inclui todos os arquivos necessários para o novo Pull Request
</commit_message>
<xml_diff>
--- a/ThemeColors/ThemeColorsCorrect.xlsx
+++ b/ThemeColors/ThemeColorsCorrect.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stuconestogacon-my.sharepoint.com/personal/dhenrique6425_conestogac_on_ca/Documents/Computer Programming 4º Term/Application Project - Capstone/Test Frontend/ThemeColors/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davihenrique/Cartbutler/frontend-categories-screen/ThemeColors/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1882A65C-6724-D74C-B402-43F83CB894DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A87DD4-A7A4-7B43-82CD-6BD93435DC7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="25600" windowHeight="14560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -617,7 +617,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="26" x14ac:dyDescent="0.3"/>

</xml_diff>